<commit_message>
Everything ready to get started; traditional process
</commit_message>
<xml_diff>
--- a/InfoComercio.xlsx
+++ b/InfoComercio.xlsx
@@ -8,17 +8,21 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agustin/Documents/Python/IntegracionVolcado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25EE362B-4FA8-454D-BF05-0A528E88D8D2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0548DFFE-5E32-FE4F-B827-FFB3BE0E1370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1200" yWindow="3380" windowWidth="25240" windowHeight="13940" xr2:uid="{97E8C2B8-B5EB-8148-BC70-754F650C5247}"/>
+    <workbookView xWindow="1300" yWindow="-17740" windowWidth="25240" windowHeight="13940" activeTab="1" xr2:uid="{97E8C2B8-B5EB-8148-BC70-754F650C5247}"/>
   </bookViews>
   <sheets>
-    <sheet name="Comercio" sheetId="1" r:id="rId1"/>
-    <sheet name="Sucursal" sheetId="2" r:id="rId2"/>
+    <sheet name="Comercio_ANT" sheetId="1" r:id="rId1"/>
+    <sheet name="Comercio" sheetId="3" r:id="rId2"/>
+    <sheet name="Sucursal" sheetId="4" r:id="rId3"/>
+    <sheet name="Sucursal_ANT" sheetId="2" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName name="Comercio" localSheetId="0">Comercio!$A$1:$AC$2</definedName>
-    <definedName name="Sucursal" localSheetId="1">Sucursal!$A$1:$J$2</definedName>
+    <definedName name="Comercio" localSheetId="0">Comercio_ANT!$A$1:$AC$2</definedName>
+    <definedName name="data_1741806207583" localSheetId="1">Comercio!$A$1:$AC$2</definedName>
+    <definedName name="data_1741806378468" localSheetId="2">Sucursal!$A$1:$J$2</definedName>
+    <definedName name="Sucursal" localSheetId="3">Sucursal_ANT!$A$1:$J$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -78,7 +82,58 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{9FB94B6B-A114-5042-82D5-0B1C0E25165D}" name="Sucursal" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="2" xr16:uid="{8F9E9F76-A639-DC4F-B460-01B00E2484BE}" name="data-1741806207583" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/agustin/Downloads/data-1741806207583.csv" tab="0" comma="1">
+      <textFields count="29">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="3" xr16:uid="{5D474BA1-CDB9-D94E-A35C-605431BD28EA}" name="data-1741806378468" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/agustin/Downloads/data-1741806378468.csv" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="4" xr16:uid="{9FB94B6B-A114-5042-82D5-0B1C0E25165D}" name="Sucursal" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/agustin/Downloads/Sucursal.csv" tab="0" comma="1">
       <textFields count="12">
         <textField/>
@@ -100,7 +155,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
   <si>
     <t>id</t>
   </si>
@@ -189,67 +244,82 @@
     <t>tipo_despacho</t>
   </si>
   <si>
-    <t>99578450-5</t>
-  </si>
-  <si>
-    <t>hpimentelc@gmail.com</t>
-  </si>
-  <si>
-    <t>KATEMU SA</t>
-  </si>
-  <si>
     <t>Teatinos 500, Santiago, METROPOLITANA</t>
   </si>
   <si>
-    <t>[{"bank": 12, "fullName": "KATEMU S.A", "ownerRut": "99578450-5", "idAccount": null, "ownerMail": "hpimentelc@gmail.com", "accountType": 3, "accountNumber": "99578450"}]</t>
-  </si>
-  <si>
-    <t>[{"names": "asdasdasd", "lastName": "asdasdas", "contactRut": "16953506-K", "contactMail": "hpimentelc@gmail.com", "contactPhone": "997910554", "contactNSerie": "121313131", "secondLastName": "asdasd"}]</t>
-  </si>
-  <si>
-    <t>[{"names": "asdasdasd", "lastName": "asdasdas", "secondLastName": "asdasd", "legalRepresentativeRUT": "16953506-K", "legalRepresentativeMail": "hpimentelc@gmail.com", "legalRepresentativePhone": "997910554", "legalRepresentativeNSerie": "121313131"}]</t>
-  </si>
-  <si>
-    <t>[{"id": 6, "code": "REGCOM", "name": "Registro de comercio", "status": 1, "createdDate": 1740079065085, "description": "El comercio acaba de ingresar en la pagina de autoafiliacion ecommerce"}, {"id": 7, "code": "REGCONT", "name": "Registro de datos de contacto", "status": 1, "createdDate": 1740079093760, "description": "El comercio ingreso los datos de contacto."}, {"id": 8, "code": "DATCOM", "name": "Datos de comercio", "status": 1, "createdDate": 1740079133212, "description": "El comercio ingreso los datos de comercio"}, {"id": 9, "code": "CTABANC", "name": "Datos de cuentas bancarias", "status": 1, "createdDate": 1740079198312, "description": "El comercio ingreso los datos de cuentas bancarias"}, {"id": 10, "code": "DOCU", "name": "Pantalla documentos", "status": 1, "createdDate": 1740081420363, "description": "El comercio ingreso los documentos necesarios"}, {"id": 11, "code": "UAF", "name": "Pantalla UAF", "status": 1, "createdDate": 1740146973211, "description": "El comercio ingreso los datos de UAF"}, {"id": 16, "code": "SUMMARY", "name": "Pantalla Resumen", "status": 1, "createdDate": 1740146979117, "description": "El comercio revisa y acepta el resumen"}]</t>
+    <t>AUTOAFILIACION_POS</t>
+  </si>
+  <si>
+    <t>AUTOAFILIACION_KLAP</t>
+  </si>
+  <si>
+    <t>RED_POS</t>
+  </si>
+  <si>
+    <t>id_comercio</t>
+  </si>
+  <si>
+    <t>terminales</t>
+  </si>
+  <si>
+    <t>servicios</t>
+  </si>
+  <si>
+    <t>configuracion_cuentas</t>
+  </si>
+  <si>
+    <t>mcc</t>
+  </si>
+  <si>
+    <t>id_giro</t>
+  </si>
+  <si>
+    <t>codigo_actividad_economica</t>
+  </si>
+  <si>
+    <t>fecha_entrega_pos</t>
+  </si>
+  <si>
+    <t>15985129-K</t>
+  </si>
+  <si>
+    <t>agustingoni@gmail.com</t>
+  </si>
+  <si>
+    <t>CESAR ISRRAEL GATICA VILLAGRAN</t>
+  </si>
+  <si>
+    <t>[{bank": 53, "fullName": "Johnny Walker Gallon", "ownerRut": "15985129-K", "idAccount": null, "ownerMail": "agustingoni@gmail.com", "accountType": 2, "accountNumber": "12345678"}]"</t>
+  </si>
+  <si>
+    <t>[{names": "Johnny", "lastName": "Walker", "contactRut": "15985129-K", "contactMail": "agustingoni@gmail.com", "contactPhone": "912345678", "contactNSerie": "123456789", "secondLastName": "Gallon"}]"</t>
+  </si>
+  <si>
+    <t>[{names": "Johnny", "lastName": "Walker", "secondLastName": "Gallon", "legalRepresentativeRUT": "15985129-K", "legalRepresentativeMail": "agustingoni@gmail.com", "legalRepresentativePhone": "912345678", "legalRepresentativeNSerie": "123456789"}]"</t>
+  </si>
+  <si>
+    <t>[{id": 6, "code": "REGCOM", "name": "Registro de comercio", "status": 1, "createdDate": 1741803470132, "description": "El comercio acaba de ingresar en la pagina de autoafiliacion ecommerce"}, {"id": 7, "code": "REGCONT", "name": "Registro de datos de contacto", "status": 1, "createdDate": 1741803501194, "description": "El comercio ingreso los datos de contacto."}, {"id": 8, "code": "DATCOM", "name": "Datos de comercio", "status": 1, "createdDate": 1741803537057, "description": "El comercio ingreso los datos de comercio"}, {"id": 9, "code": "CTABANC", "name": "Datos de cuentas bancarias", "status": 1, "createdDate": 1741803558012, "description": "El comercio ingreso los datos de cuentas bancarias"}, {"id": 10, "code": "DOCU", "name": "Pantalla documentos", "status": 1, "createdDate": 1741803607577, "description": "El comercio ingreso los documentos necesarios"}, {"id": 16, "code": "SUMMARY", "name": "Pantalla Resumen", "status": 1, "createdDate": 1741803613147, "description": "El comercio revisa y acepta el resumen"}]"</t>
+  </si>
+  <si>
+    <t>[{idCore": 21, "transactionType": "Venta"}]"</t>
+  </si>
+  <si>
+    <t>[{idCore": 4, "serviceType": "pos", "idServiceAYC": null, "configuration": null, "integrationType": "movistar"}]"</t>
+  </si>
+  <si>
+    <t>[{"bank": 53, "fullName": "Johnny Walker Gallon", "ownerRut": "15985129-K", "idAccount": null, "ownerMail": "agustingoni@gmail.com", "accountType": 2, "accountNumber": "12345678"}]</t>
+  </si>
+  <si>
+    <t>[{"names": "Johnny", "lastName": "Walker", "contactRut": "15985129-K", "contactMail": "agustingoni@gmail.com", "contactPhone": "912345678", "contactNSerie": "123456789", "secondLastName": "Gallon"}]</t>
+  </si>
+  <si>
+    <t>[{"names": "Johnny", "lastName": "Walker", "secondLastName": "Gallon", "legalRepresentativeRUT": "15985129-K", "legalRepresentativeMail": "agustingoni@gmail.com", "legalRepresentativePhone": "912345678", "legalRepresentativeNSerie": "123456789"}]</t>
+  </si>
+  <si>
+    <t>[{"id": 6, "code": "REGCOM", "name": "Registro de comercio", "status": 1, "createdDate": 1741803470132, "description": "El comercio acaba de ingresar en la pagina de autoafiliacion ecommerce"}, {"id": 7, "code": "REGCONT", "name": "Registro de datos de contacto", "status": 1, "createdDate": 1741803501194, "description": "El comercio ingreso los datos de contacto."}, {"id": 8, "code": "DATCOM", "name": "Datos de comercio", "status": 1, "createdDate": 1741803537057, "description": "El comercio ingreso los datos de comercio"}, {"id": 9, "code": "CTABANC", "name": "Datos de cuentas bancarias", "status": 1, "createdDate": 1741803558012, "description": "El comercio ingreso los datos de cuentas bancarias"}, {"id": 10, "code": "DOCU", "name": "Pantalla documentos", "status": 1, "createdDate": 1741803607577, "description": "El comercio ingreso los documentos necesarios"}, {"id": 16, "code": "SUMMARY", "name": "Pantalla Resumen", "status": 1, "createdDate": 1741803613147, "description": "El comercio revisa y acepta el resumen"}]</t>
   </si>
   <si>
     <t>NULL</t>
-  </si>
-  <si>
-    <t>{"relation": "Representante legal", "entityType": "An√≥nima", "nationality": "Chilena", "originPlace": "CHILE", "efectiveControl": [{"cni": "11111111-1", "city": "asdasdasd", "address": "asdasd", "country": "CHILE", "fullName": "asdasd", "participation": 100}], "finalBeneficiary": [{"cni": "11111111-1", "city": "asdasdasd", "address": "asdasd", "country": "CHILE", "fullName": "asdasd", "participation": 100}], "countryConstitution": "CHILE"}</t>
-  </si>
-  <si>
-    <t>AUTOAFILIACION_POS</t>
-  </si>
-  <si>
-    <t>AUTOAFILIACION_KLAP</t>
-  </si>
-  <si>
-    <t>RED_POS</t>
-  </si>
-  <si>
-    <t>id_comercio</t>
-  </si>
-  <si>
-    <t>terminales</t>
-  </si>
-  <si>
-    <t>servicios</t>
-  </si>
-  <si>
-    <t>configuracion_cuentas</t>
-  </si>
-  <si>
-    <t>mcc</t>
-  </si>
-  <si>
-    <t>id_giro</t>
-  </si>
-  <si>
-    <t>codigo_actividad_economica</t>
-  </si>
-  <si>
-    <t>fecha_entrega_pos</t>
   </si>
   <si>
     <t>[{"idCore": 21, "transactionType": "Venta"}]</t>
@@ -317,7 +387,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Sucursal" connectionId="2" xr16:uid="{5279BB64-A961-0740-A871-AAB12BD4F753}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data-1741806207583" connectionId="2" xr16:uid="{73DB1582-B341-0F46-B5FE-E05185FC83CF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data-1741806378468" connectionId="3" xr16:uid="{EE77210E-2AD2-FE4C-BBFF-D93519A1027F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Sucursal" connectionId="4" xr16:uid="{5279BB64-A961-0740-A871-AAB12BD4F753}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -639,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FD856DD2-7071-9D47-875C-3929C8B88AC0}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -764,55 +842,46 @@
     </row>
     <row r="2" spans="1:29" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>1075</v>
+        <v>1112</v>
       </c>
       <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
         <v>29</v>
       </c>
-      <c r="C2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D2" t="s">
-        <v>31</v>
-      </c>
-      <c r="E2" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" t="s">
-        <v>32</v>
-      </c>
       <c r="G2">
-        <v>535</v>
+        <v>352</v>
       </c>
       <c r="H2" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="I2" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="J2" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="K2" t="s">
-        <v>36</v>
+        <v>47</v>
       </c>
       <c r="L2" s="1">
-        <v>45708.678994004629</v>
+        <v>45728.637385752314</v>
       </c>
       <c r="M2">
         <v>1</v>
       </c>
       <c r="N2" s="1">
-        <v>45708.706254201388</v>
-      </c>
-      <c r="O2" t="s">
-        <v>37</v>
-      </c>
-      <c r="P2" t="s">
-        <v>38</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>37</v>
+        <v>45728.638976585651</v>
       </c>
       <c r="R2">
         <v>70</v>
@@ -824,31 +893,22 @@
         <v>0</v>
       </c>
       <c r="U2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="V2">
-        <v>997910554</v>
-      </c>
-      <c r="W2" t="s">
-        <v>37</v>
+        <v>912345678</v>
       </c>
       <c r="X2" t="b">
         <v>0</v>
       </c>
-      <c r="Y2" t="s">
-        <v>37</v>
-      </c>
       <c r="Z2" s="2">
         <v>45662</v>
       </c>
       <c r="AA2" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="AC2" t="s">
-        <v>41</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -857,11 +917,231 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAB8CCD-9CF7-3845-AF8B-C1AAF2646F63}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB59D71-39F3-9346-B2E6-7B47353AD1EC}">
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AB2" sqref="AB2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="29.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1112</v>
+      </c>
+      <c r="B2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>352</v>
+      </c>
+      <c r="H2" t="s">
+        <v>50</v>
+      </c>
+      <c r="I2" t="s">
+        <v>51</v>
+      </c>
+      <c r="J2" t="s">
+        <v>52</v>
+      </c>
+      <c r="K2" t="s">
+        <v>53</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45728.637385752314</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45728.638976585651</v>
+      </c>
+      <c r="O2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2">
+        <v>70</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2">
+        <v>912345678</v>
+      </c>
+      <c r="W2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>45662</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E86D6628-55A9-6C4C-9C69-3256A0A67A91}">
   <dimension ref="A1:J2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -883,63 +1163,148 @@
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>42</v>
+        <v>33</v>
       </c>
       <c r="C1" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
       <c r="D1" t="s">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="E1" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="F1" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="G1" t="s">
         <v>12</v>
       </c>
       <c r="H1" t="s">
-        <v>47</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>48</v>
+        <v>39</v>
       </c>
       <c r="J1" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>639</v>
+        <v>650</v>
       </c>
       <c r="B2">
-        <v>1075</v>
+        <v>1112</v>
       </c>
       <c r="C2" t="s">
-        <v>50</v>
+        <v>55</v>
       </c>
       <c r="D2" t="s">
-        <v>51</v>
+        <v>56</v>
       </c>
       <c r="E2" t="s">
-        <v>37</v>
+        <v>54</v>
       </c>
       <c r="F2">
-        <v>4</v>
+        <v>190</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
       <c r="H2">
-        <v>535</v>
+        <v>352</v>
       </c>
       <c r="I2">
-        <v>410010</v>
+        <v>960909</v>
       </c>
       <c r="J2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAB8CCD-9CF7-3845-AF8B-C1AAF2646F63}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
         <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>650</v>
+      </c>
+      <c r="B2">
+        <v>1112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2">
+        <v>190</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>352</v>
+      </c>
+      <c r="I2">
+        <v>960909</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Ready to start comprehensive testing
</commit_message>
<xml_diff>
--- a/InfoComercio.xlsx
+++ b/InfoComercio.xlsx
@@ -8,21 +8,25 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agustin/Documents/Python/IntegracionVolcado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0548DFFE-5E32-FE4F-B827-FFB3BE0E1370}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12730663-8704-2748-99DC-01CA5BD6F119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1300" yWindow="-17740" windowWidth="25240" windowHeight="13940" activeTab="1" xr2:uid="{97E8C2B8-B5EB-8148-BC70-754F650C5247}"/>
+    <workbookView xWindow="6280" yWindow="6140" windowWidth="25240" windowHeight="13940" activeTab="4" xr2:uid="{97E8C2B8-B5EB-8148-BC70-754F650C5247}"/>
   </bookViews>
   <sheets>
     <sheet name="Comercio_ANT" sheetId="1" r:id="rId1"/>
-    <sheet name="Comercio" sheetId="3" r:id="rId2"/>
-    <sheet name="Sucursal" sheetId="4" r:id="rId3"/>
-    <sheet name="Sucursal_ANT" sheetId="2" r:id="rId4"/>
+    <sheet name="Comercio_ANT1" sheetId="3" r:id="rId2"/>
+    <sheet name="Sucursal_ANT1" sheetId="4" r:id="rId3"/>
+    <sheet name="Comercio" sheetId="5" r:id="rId4"/>
+    <sheet name="Sucursal" sheetId="6" r:id="rId5"/>
+    <sheet name="Sucursal_ANT" sheetId="2" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="Comercio" localSheetId="0">Comercio_ANT!$A$1:$AC$2</definedName>
-    <definedName name="data_1741806207583" localSheetId="1">Comercio!$A$1:$AC$2</definedName>
-    <definedName name="data_1741806378468" localSheetId="2">Sucursal!$A$1:$J$2</definedName>
-    <definedName name="Sucursal" localSheetId="3">Sucursal_ANT!$A$1:$J$2</definedName>
+    <definedName name="data_1741806207583" localSheetId="1">Comercio_ANT1!$A$1:$AC$2</definedName>
+    <definedName name="data_1741806378468" localSheetId="2">Sucursal_ANT1!$A$1:$J$2</definedName>
+    <definedName name="data_1741958763025" localSheetId="3">Comercio!$A$1:$AC$2</definedName>
+    <definedName name="data_1741959077358" localSheetId="4">Sucursal!$A$1:$J$2</definedName>
+    <definedName name="Sucursal" localSheetId="5">Sucursal_ANT!$A$1:$J$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -133,7 +137,59 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{9FB94B6B-A114-5042-82D5-0B1C0E25165D}" name="Sucursal" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="4" xr16:uid="{151ACC7E-7D0B-474E-9A7E-CC17457D8605}" name="data-1741958763025" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/agustin/Downloads/data-1741958763025.csv" comma="1">
+      <textFields count="30">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="5" xr16:uid="{ED10C2D2-3C4D-174C-9A56-7F73B5F143C2}" name="data-1741959077358" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/agustin/Downloads/data-1741959077358.csv" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="6" xr16:uid="{9FB94B6B-A114-5042-82D5-0B1C0E25165D}" name="Sucursal" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/agustin/Downloads/Sucursal.csv" tab="0" comma="1">
       <textFields count="12">
         <textField/>
@@ -155,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="114" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="63">
   <si>
     <t>id</t>
   </si>
@@ -326,6 +382,24 @@
   </si>
   <si>
     <t>[{"idCore": 4, "serviceType": "pos", "idServiceAYC": null, "configuration": null, "integrationType": "movistar"}]</t>
+  </si>
+  <si>
+    <t>13604300-5</t>
+  </si>
+  <si>
+    <t>CLAUDIA SOLEDAD INZUNZA BRAVO</t>
+  </si>
+  <si>
+    <t>[{"bank": 16, "fullName": "Gonzalo Gonzalez Reiterado", "ownerRut": "13604300-5", "idAccount": null, "ownerMail": "agustingoni@gmail.com", "accountType": 2, "accountNumber": "12346532"}]</t>
+  </si>
+  <si>
+    <t>[{"names": "Gonzalo", "lastName": "Gonzalez", "contactRut": "13604300-5", "contactMail": "agustingoni@gmail.com", "contactPhone": "912345678", "contactNSerie": "123456789", "secondLastName": "Reiterado"}]</t>
+  </si>
+  <si>
+    <t>[{"names": "Gonzalo", "lastName": "Gonzalez", "secondLastName": "Reiterado", "legalRepresentativeRUT": "13604300-5", "legalRepresentativeMail": "agustingoni@gmail.com", "legalRepresentativePhone": "912345678", "legalRepresentativeNSerie": "123456789"}]</t>
+  </si>
+  <si>
+    <t>[{"id": 6, "code": "REGCOM", "name": "Registro de comercio", "status": 1, "createdDate": 1741958344237, "description": "El comercio acaba de ingresar en la pagina de autoafiliacion ecommerce"}, {"id": 7, "code": "REGCONT", "name": "Registro de datos de contacto", "status": 1, "createdDate": 1741958389978, "description": "El comercio ingreso los datos de contacto."}, {"id": 8, "code": "DATCOM", "name": "Datos de comercio", "status": 1, "createdDate": 1741958414986, "description": "El comercio ingreso los datos de comercio"}, {"id": 9, "code": "CTABANC", "name": "Datos de cuentas bancarias", "status": 1, "createdDate": 1741958442031, "description": "El comercio ingreso los datos de cuentas bancarias"}, {"id": 10, "code": "DOCU", "name": "Pantalla documentos", "status": 1, "createdDate": 1741958496224, "description": "El comercio ingreso los documentos necesarios"}, {"id": 16, "code": "SUMMARY", "name": "Pantalla Resumen", "status": 1, "createdDate": 1741958508152, "description": "El comercio revisa y acepta el resumen"}]</t>
   </si>
 </sst>
 </file>
@@ -395,7 +469,15 @@
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Sucursal" connectionId="4" xr16:uid="{5279BB64-A961-0740-A871-AAB12BD4F753}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data-1741958763025" connectionId="4" xr16:uid="{567217C8-310A-9644-BEAF-DD3B74F99FE8}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data-1741959077358" connectionId="5" xr16:uid="{0257A10C-FFFE-CE4E-88F7-3C8184CC6705}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Sucursal" connectionId="6" xr16:uid="{5279BB64-A961-0740-A871-AAB12BD4F753}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -920,8 +1002,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB59D71-39F3-9346-B2E6-7B47353AD1EC}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AB2" sqref="AB2"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1228,10 +1310,321 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539F3129-0E8B-BC4D-B356-59FC33B4A44F}">
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="AD8" sqref="AD8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1113</v>
+      </c>
+      <c r="B2" t="s">
+        <v>57</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>58</v>
+      </c>
+      <c r="E2" t="s">
+        <v>58</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>352</v>
+      </c>
+      <c r="H2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" t="s">
+        <v>60</v>
+      </c>
+      <c r="J2" t="s">
+        <v>61</v>
+      </c>
+      <c r="K2" t="s">
+        <v>62</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45730.429910127314</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45730.431669259262</v>
+      </c>
+      <c r="O2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2">
+        <v>70</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2">
+        <v>912345678</v>
+      </c>
+      <c r="W2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" s="2">
+        <v>45662</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD7088C-55B7-9F45-85FC-35A54B40E2DF}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="K1" sqref="K1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>651</v>
+      </c>
+      <c r="B2">
+        <v>1113</v>
+      </c>
+      <c r="C2" t="s">
+        <v>55</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2">
+        <v>190</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>352</v>
+      </c>
+      <c r="I2">
+        <v>960909</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAB8CCD-9CF7-3845-AF8B-C1AAF2646F63}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Closing the day... so far
</commit_message>
<xml_diff>
--- a/InfoComercio.xlsx
+++ b/InfoComercio.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agustin/Documents/Python/IntegracionVolcado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12730663-8704-2748-99DC-01CA5BD6F119}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF38FED6-4C45-194C-A9AC-FB3D6284D274}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="6140" windowWidth="25240" windowHeight="13940" activeTab="4" xr2:uid="{97E8C2B8-B5EB-8148-BC70-754F650C5247}"/>
+    <workbookView xWindow="6280" yWindow="6140" windowWidth="25240" windowHeight="13940" activeTab="3" xr2:uid="{97E8C2B8-B5EB-8148-BC70-754F650C5247}"/>
   </bookViews>
   <sheets>
     <sheet name="Comercio_ANT" sheetId="1" r:id="rId1"/>
@@ -211,7 +211,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="176" uniqueCount="64">
   <si>
     <t>id</t>
   </si>
@@ -400,6 +400,9 @@
   </si>
   <si>
     <t>[{"id": 6, "code": "REGCOM", "name": "Registro de comercio", "status": 1, "createdDate": 1741958344237, "description": "El comercio acaba de ingresar en la pagina de autoafiliacion ecommerce"}, {"id": 7, "code": "REGCONT", "name": "Registro de datos de contacto", "status": 1, "createdDate": 1741958389978, "description": "El comercio ingreso los datos de contacto."}, {"id": 8, "code": "DATCOM", "name": "Datos de comercio", "status": 1, "createdDate": 1741958414986, "description": "El comercio ingreso los datos de comercio"}, {"id": 9, "code": "CTABANC", "name": "Datos de cuentas bancarias", "status": 1, "createdDate": 1741958442031, "description": "El comercio ingreso los datos de cuentas bancarias"}, {"id": 10, "code": "DOCU", "name": "Pantalla documentos", "status": 1, "createdDate": 1741958496224, "description": "El comercio ingreso los documentos necesarios"}, {"id": 16, "code": "SUMMARY", "name": "Pantalla Resumen", "status": 1, "createdDate": 1741958508152, "description": "El comercio revisa y acepta el resumen"}]</t>
+  </si>
+  <si>
+    <t>9743043-8</t>
   </si>
 </sst>
 </file>
@@ -1002,8 +1005,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB59D71-39F3-9346-B2E6-7B47353AD1EC}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="AC1" sqref="AC1"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1313,8 +1316,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539F3129-0E8B-BC4D-B356-59FC33B4A44F}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="AD8" sqref="AD8"/>
+    <sheetView tabSelected="1" topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Z2" sqref="Z2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1511,8 +1514,8 @@
       <c r="Y2" t="s">
         <v>54</v>
       </c>
-      <c r="Z2" s="2">
-        <v>45662</v>
+      <c r="Z2" s="2" t="s">
+        <v>63</v>
       </c>
       <c r="AA2" t="s">
         <v>31</v>
@@ -1533,7 +1536,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD7088C-55B7-9F45-85FC-35A54B40E2DF}">
   <dimension ref="A1:J2"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Probado con PN y PJ
</commit_message>
<xml_diff>
--- a/InfoComercio.xlsx
+++ b/InfoComercio.xlsx
@@ -8,25 +8,33 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/agustin/Documents/Python/IntegracionVolcado/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7E7F9E92-90D4-4042-BF45-8A07D8E92AD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{003E9D1E-7DB3-A746-B01D-2DB31C2D03DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6280" yWindow="6140" windowWidth="25240" windowHeight="13940" activeTab="4" xr2:uid="{97E8C2B8-B5EB-8148-BC70-754F650C5247}"/>
+    <workbookView xWindow="6280" yWindow="6140" windowWidth="25240" windowHeight="13940" activeTab="8" xr2:uid="{97E8C2B8-B5EB-8148-BC70-754F650C5247}"/>
   </bookViews>
   <sheets>
     <sheet name="Comercio_ANT" sheetId="1" r:id="rId1"/>
     <sheet name="Comercio_ANT1" sheetId="3" r:id="rId2"/>
     <sheet name="Sucursal_ANT1" sheetId="4" r:id="rId3"/>
-    <sheet name="Comercio" sheetId="5" r:id="rId4"/>
-    <sheet name="Sucursal" sheetId="6" r:id="rId5"/>
-    <sheet name="Sucursal_ANT" sheetId="2" r:id="rId6"/>
+    <sheet name="Comercio_BCK" sheetId="5" r:id="rId4"/>
+    <sheet name="Sucursal_BCK" sheetId="6" r:id="rId5"/>
+    <sheet name="Comercio_BCK2" sheetId="7" r:id="rId6"/>
+    <sheet name="Sucursal_BCK2" sheetId="8" r:id="rId7"/>
+    <sheet name="Comercio" sheetId="9" r:id="rId8"/>
+    <sheet name="Sucursal" sheetId="10" r:id="rId9"/>
+    <sheet name="Sucursal_ANT" sheetId="2" r:id="rId10"/>
   </sheets>
   <definedNames>
     <definedName name="Comercio" localSheetId="0">Comercio_ANT!$A$1:$AC$2</definedName>
     <definedName name="data_1741806207583" localSheetId="1">Comercio_ANT1!$A$1:$AC$2</definedName>
     <definedName name="data_1741806378468" localSheetId="2">Sucursal_ANT1!$A$1:$J$2</definedName>
-    <definedName name="data_1741958763025" localSheetId="3">Comercio!$A$1:$AC$2</definedName>
-    <definedName name="data_1741959077358" localSheetId="4">Sucursal!$A$1:$J$2</definedName>
-    <definedName name="Sucursal" localSheetId="5">Sucursal_ANT!$A$1:$J$2</definedName>
+    <definedName name="data_1741958763025" localSheetId="3">Comercio_BCK!$A$1:$AC$2</definedName>
+    <definedName name="data_1741959077358" localSheetId="4">Sucursal_BCK!$A$1:$J$2</definedName>
+    <definedName name="data_1742484287298" localSheetId="5">Comercio_BCK2!$A$1:$AC$2</definedName>
+    <definedName name="data_1742484447339" localSheetId="6">Sucursal_BCK2!$A$1:$J$2</definedName>
+    <definedName name="data_1742499068268" localSheetId="7">Comercio!$A$1:$AC$2</definedName>
+    <definedName name="data_1742499210440" localSheetId="8">Sucursal!$A$1:$J$2</definedName>
+    <definedName name="Sucursal" localSheetId="9">Sucursal_ANT!$A$1:$J$2</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -189,7 +197,109 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="6" xr16:uid="{9FB94B6B-A114-5042-82D5-0B1C0E25165D}" name="Sucursal" type="6" refreshedVersion="8" background="1" saveData="1">
+  <connection id="6" xr16:uid="{5BCDB35D-C564-E140-B46C-6A4E5AF62F3B}" name="data-1742484287298" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/agustin/Downloads/data-1742484287298.csv" comma="1">
+      <textFields count="29">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="7" xr16:uid="{1D84AADE-FDB2-964D-AF65-537104EA6B14}" name="data-1742484447339" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr sourceFile="/Users/agustin/Downloads/data-1742484447339.csv" tab="0" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="8" xr16:uid="{45F49B92-B994-8545-AE84-0B5D8F9EDD62}" name="data-1742499068268" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/agustin/Downloads/data-1742499068268.csv" tab="0" comma="1">
+      <textFields count="29">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="9" xr16:uid="{50EA4399-3BCB-BE43-BBAA-679A00FB33F1}" name="data-1742499210440" type="6" refreshedVersion="8" background="1" saveData="1">
+    <textPr codePage="10000" sourceFile="/Users/agustin/Downloads/data-1742499210440.csv" tab="0" comma="1">
+      <textFields count="10">
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+        <textField/>
+      </textFields>
+    </textPr>
+  </connection>
+  <connection id="10" xr16:uid="{9FB94B6B-A114-5042-82D5-0B1C0E25165D}" name="Sucursal" type="6" refreshedVersion="8" background="1" saveData="1">
     <textPr sourceFile="/Users/agustin/Downloads/Sucursal.csv" tab="0" comma="1">
       <textFields count="12">
         <textField/>
@@ -211,7 +321,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="180" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="81">
   <si>
     <t>id</t>
   </si>
@@ -409,6 +519,51 @@
   </si>
   <si>
     <t>[{"idCore": 21, "transactionType": "Venta"}, {"idCore": 21, "transactionType": "Venta"}]</t>
+  </si>
+  <si>
+    <t>11574234-5</t>
+  </si>
+  <si>
+    <t>JEANNETTE ELVIRA MATAMALA ARROYO</t>
+  </si>
+  <si>
+    <t>[{"bank": 27, "fullName": "Juanito Barroga Delgado", "ownerRut": "11574234-5", "idAccount": null, "ownerMail": "agustingoni@gmail.com", "accountType": 2, "accountNumber": "456456789"}]</t>
+  </si>
+  <si>
+    <t>[{"names": "Juanito", "lastName": "Barroga", "contactRut": "11574234-5", "contactMail": "agustingoni@gmail.com", "contactPhone": "912345678", "contactNSerie": "123123123", "secondLastName": "Delgado"}]</t>
+  </si>
+  <si>
+    <t>[{"names": "Juanito", "lastName": "Barroga", "secondLastName": "Delgado", "legalRepresentativeRUT": "11574234-5", "legalRepresentativeMail": "agustingoni@gmail.com", "legalRepresentativePhone": "912345678", "legalRepresentativeNSerie": "123123123"}]</t>
+  </si>
+  <si>
+    <t>[{"id": 6, "code": "REGCOM", "name": "Registro de comercio", "status": 1, "createdDate": 1742473722353, "description": "El comercio acaba de ingresar en la pagina de autoafiliacion ecommerce"}, {"id": 7, "code": "REGCONT", "name": "Registro de datos de contacto", "status": 1, "createdDate": 1742474475861, "description": "El comercio ingreso los datos de contacto."}, {"id": 8, "code": "DATCOM", "name": "Datos de comercio", "status": 1, "createdDate": 1742474506580, "description": "El comercio ingreso los datos de comercio"}, {"id": 9, "code": "CTABANC", "name": "Datos de cuentas bancarias", "status": 1, "createdDate": 1742474527660, "description": "El comercio ingreso los datos de cuentas bancarias"}, {"id": 10, "code": "DOCU", "name": "Pantalla documentos", "status": 1, "createdDate": 1742474567355, "description": "El comercio ingreso los documentos necesarios"}, {"id": 16, "code": "SUMMARY", "name": "Pantalla Resumen", "status": 1, "createdDate": 1742474710734, "description": "El comercio revisa y acepta el resumen"}]</t>
+  </si>
+  <si>
+    <t>[{"idCore": 21, "transactionType": "Venta"}, {"idCore": 21, "transactionType": "Venta"}, {"idCore": 21, "transactionType": "Venta"}, {"idCore": 21, "transactionType": "Venta"}]</t>
+  </si>
+  <si>
+    <t>76073162-5</t>
+  </si>
+  <si>
+    <t>SOCIEDAD AUSTRAL DE ELECTRICIDAD SA</t>
+  </si>
+  <si>
+    <t>CONCEPCION 120, PUERTO MONTT, DE LOS LAGOS, Puerto Montt</t>
+  </si>
+  <si>
+    <t>[{"bank": 37, "fullName": "SOCIEDAD AUSTRAL DE ELECTRICIDAD S.A.", "ownerRut": "76073162-5", "idAccount": null, "ownerMail": "agustingoni@gmail.com", "accountType": 2, "accountNumber": "1231231231"}]</t>
+  </si>
+  <si>
+    <t>[{"names": "Veronica", "lastName": "Merino", "contactRut": "12077264-3", "contactMail": "agustingoni@gmail.com", "contactPhone": "912345678", "contactNSerie": "123123132", "secondLastName": "Vidal"}]</t>
+  </si>
+  <si>
+    <t>[{"names": "Veronica", "lastName": "Merino", "secondLastName": "Vidal", "legalRepresentativeRUT": "12077264-3", "legalRepresentativeMail": "agustingoni@gmail.com", "legalRepresentativePhone": "912345678", "legalRepresentativeNSerie": "123123132"}]</t>
+  </si>
+  <si>
+    <t>[{"id": 6, "code": "REGCOM", "name": "Registro de comercio", "status": 1, "createdDate": 1742475473195, "description": "El comercio acaba de ingresar en la pagina de autoafiliacion ecommerce"}, {"id": 7, "code": "REGCONT", "name": "Registro de datos de contacto", "status": 1, "createdDate": 1742475535945, "description": "El comercio ingreso los datos de contacto."}, {"id": 8, "code": "DATCOM", "name": "Datos de comercio", "status": 1, "createdDate": 1742475595509, "description": "El comercio ingreso los datos de comercio"}, {"id": 9, "code": "CTABANC", "name": "Datos de cuentas bancarias", "status": 1, "createdDate": 1742475610235, "description": "El comercio ingreso los datos de cuentas bancarias"}, {"id": 10, "code": "DOCU", "name": "Pantalla documentos", "status": 1, "createdDate": 1742475652020, "description": "El comercio ingreso los documentos necesarios"}, {"id": 11, "code": "UAF", "name": "Pantalla UAF", "status": 1, "createdDate": 1742475710658, "description": "El comercio ingreso los datos de UAF"}, {"id": 16, "code": "SUMMARY", "name": "Pantalla Resumen", "status": 1, "createdDate": 1742475749544, "description": "El comercio revisa y acepta el resumen"}]</t>
+  </si>
+  <si>
+    <t>{"relation": "Representante legal", "entityType": "An√≥nima", "nationality": "Chilena", "originPlace": "CHILE", "efectiveControl": [{"cni": "14438381-8", "city": "Lara", "address": "Mu√±oz", "country": "CHILE", "fullName": "Jorge", "participation": 100}], "finalBeneficiary": [{"cni": "14438381-8", "city": "Lara", "address": "Mu√±oz", "country": "CHILE", "fullName": "Jorge", "participation": 100}], "countryConstitution": "CHILE"}</t>
   </si>
 </sst>
 </file>
@@ -444,10 +599,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="47" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,6 +625,10 @@
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Comercio" connectionId="1" xr16:uid="{4F1D07B3-2ABE-D64A-BBDA-76124A3E581C}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Sucursal" connectionId="10" xr16:uid="{5279BB64-A961-0740-A871-AAB12BD4F753}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data-1741806207583" connectionId="2" xr16:uid="{73DB1582-B341-0F46-B5FE-E05185FC83CF}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
@@ -486,7 +646,19 @@
 </file>
 
 <file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="Sucursal" connectionId="6" xr16:uid="{5279BB64-A961-0740-A871-AAB12BD4F753}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data-1742484287298" connectionId="6" xr16:uid="{D04BF033-DDB5-C64E-883A-4775B9A96DCC}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data-1742484447339" connectionId="7" xr16:uid="{DDAE3B40-E5B0-C441-9C94-6781B1370378}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data-1742499068268" connectionId="8" xr16:uid="{F6AEF2E7-B416-B14C-8F57-306F91F098D1}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="data-1742499210440" connectionId="9" xr16:uid="{3EF22E0B-4BC6-9145-9D53-F33744FF0C0A}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1007,6 +1179,91 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAB8CCD-9CF7-3845-AF8B-C1AAF2646F63}">
+  <dimension ref="A1:J2"/>
+  <sheetViews>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.6640625" customWidth="1"/>
+    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>650</v>
+      </c>
+      <c r="B2">
+        <v>1112</v>
+      </c>
+      <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>49</v>
+      </c>
+      <c r="F2">
+        <v>190</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>352</v>
+      </c>
+      <c r="I2">
+        <v>960909</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EAB59D71-39F3-9346-B2E6-7B47353AD1EC}">
   <dimension ref="A1:AC2"/>
@@ -1322,8 +1579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{539F3129-0E8B-BC4D-B356-59FC33B4A44F}">
   <dimension ref="A1:AC2"/>
   <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z2" sqref="Z2"/>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="A1:AC1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1542,7 +1799,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FFD7088C-55B7-9F45-85FC-35A54B40E2DF}">
   <dimension ref="A1:J3"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
@@ -1662,11 +1919,231 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3AAB8CCD-9CF7-3845-AF8B-C1AAF2646F63}">
-  <dimension ref="A1:J2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F16282E5-65DB-A248-B45C-8DA2D457D771}">
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView topLeftCell="Q1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="33" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="34.33203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.33203125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1116</v>
+      </c>
+      <c r="B2" t="s">
+        <v>66</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="E2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
+        <v>29</v>
+      </c>
+      <c r="G2">
+        <v>352</v>
+      </c>
+      <c r="H2" t="s">
+        <v>68</v>
+      </c>
+      <c r="I2" t="s">
+        <v>69</v>
+      </c>
+      <c r="J2" t="s">
+        <v>70</v>
+      </c>
+      <c r="K2" t="s">
+        <v>71</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45736.39493451389</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45736.404714756944</v>
+      </c>
+      <c r="O2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2">
+        <v>70</v>
+      </c>
+      <c r="S2">
+        <v>13</v>
+      </c>
+      <c r="T2" t="b">
+        <v>0</v>
+      </c>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2">
+        <v>912345678</v>
+      </c>
+      <c r="W2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{47E45872-6159-0B4F-8D06-07D1AD507AFD}">
+  <dimension ref="A1:J3"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17"/>
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1677,8 +2154,8 @@
     <col min="4" max="4" width="80.6640625" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.6640625" customWidth="1"/>
-    <col min="8" max="8" width="21.83203125" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
   </cols>
@@ -1717,16 +2194,19 @@
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>650</v>
+        <v>652</v>
       </c>
       <c r="B2">
-        <v>1112</v>
+        <v>1116</v>
       </c>
       <c r="C2" t="s">
-        <v>48</v>
+        <v>65</v>
       </c>
       <c r="D2" t="s">
-        <v>49</v>
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
       </c>
       <c r="F2">
         <v>190</v>
@@ -1739,6 +2219,416 @@
       </c>
       <c r="I2">
         <v>960909</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>653</v>
+      </c>
+      <c r="B3">
+        <v>1116</v>
+      </c>
+      <c r="C3" t="s">
+        <v>72</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3">
+        <v>190</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>352</v>
+      </c>
+      <c r="I3">
+        <v>960909</v>
+      </c>
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{35745AFB-D571-6B42-9110-7E01AB3359E4}">
+  <dimension ref="A1:AC2"/>
+  <sheetViews>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="Z3" sqref="Z3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="5.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="55" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="23.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="18.1640625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="19" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="7.6640625" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="19.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.1640625" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="13" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" t="s">
+        <v>18</v>
+      </c>
+      <c r="T1" t="s">
+        <v>19</v>
+      </c>
+      <c r="U1" t="s">
+        <v>20</v>
+      </c>
+      <c r="V1" t="s">
+        <v>21</v>
+      </c>
+      <c r="W1" t="s">
+        <v>22</v>
+      </c>
+      <c r="X1" t="s">
+        <v>23</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z1" t="s">
+        <v>25</v>
+      </c>
+      <c r="AA1" t="s">
+        <v>26</v>
+      </c>
+      <c r="AB1" t="s">
+        <v>27</v>
+      </c>
+      <c r="AC1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:29" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>1117</v>
+      </c>
+      <c r="B2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D2" t="s">
+        <v>74</v>
+      </c>
+      <c r="E2" t="s">
+        <v>74</v>
+      </c>
+      <c r="F2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G2">
+        <v>431</v>
+      </c>
+      <c r="H2" t="s">
+        <v>76</v>
+      </c>
+      <c r="I2" t="s">
+        <v>77</v>
+      </c>
+      <c r="J2" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" t="s">
+        <v>79</v>
+      </c>
+      <c r="L2" s="1">
+        <v>45736.415198993054</v>
+      </c>
+      <c r="M2">
+        <v>1</v>
+      </c>
+      <c r="N2" s="1">
+        <v>45736.417268750003</v>
+      </c>
+      <c r="O2" t="s">
+        <v>54</v>
+      </c>
+      <c r="P2" t="s">
+        <v>80</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>54</v>
+      </c>
+      <c r="R2">
+        <v>261</v>
+      </c>
+      <c r="S2">
+        <v>10</v>
+      </c>
+      <c r="T2" t="b">
+        <v>1</v>
+      </c>
+      <c r="U2" t="s">
+        <v>30</v>
+      </c>
+      <c r="V2">
+        <v>912345678</v>
+      </c>
+      <c r="W2" t="s">
+        <v>54</v>
+      </c>
+      <c r="X2" t="b">
+        <v>0</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>31</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>54</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B48CD2C4-813B-4F4D-B658-3E33F0EE34BF}">
+  <dimension ref="A1:J4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="4.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="80.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="19.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="4.6640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="16.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D1" t="s">
+        <v>35</v>
+      </c>
+      <c r="E1" t="s">
+        <v>36</v>
+      </c>
+      <c r="F1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" t="s">
+        <v>12</v>
+      </c>
+      <c r="H1" t="s">
+        <v>38</v>
+      </c>
+      <c r="I1" t="s">
+        <v>39</v>
+      </c>
+      <c r="J1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2">
+        <v>653</v>
+      </c>
+      <c r="B2">
+        <v>1117</v>
+      </c>
+      <c r="C2" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" t="s">
+        <v>56</v>
+      </c>
+      <c r="E2" t="s">
+        <v>54</v>
+      </c>
+      <c r="F2">
+        <v>39</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>431</v>
+      </c>
+      <c r="I2">
+        <v>351030</v>
+      </c>
+      <c r="J2" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3">
+        <v>654</v>
+      </c>
+      <c r="B3">
+        <v>1117</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
+        <v>56</v>
+      </c>
+      <c r="E3" t="s">
+        <v>54</v>
+      </c>
+      <c r="F3">
+        <v>39</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>431</v>
+      </c>
+      <c r="I3">
+        <v>351030</v>
+      </c>
+      <c r="J3" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>655</v>
+      </c>
+      <c r="B4">
+        <v>1117</v>
+      </c>
+      <c r="C4" t="s">
+        <v>72</v>
+      </c>
+      <c r="D4" t="s">
+        <v>56</v>
+      </c>
+      <c r="E4" t="s">
+        <v>54</v>
+      </c>
+      <c r="F4">
+        <v>39</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+      <c r="H4">
+        <v>431</v>
+      </c>
+      <c r="I4">
+        <v>351030</v>
+      </c>
+      <c r="J4" t="s">
+        <v>54</v>
       </c>
     </row>
   </sheetData>

</xml_diff>